<commit_message>
Add interpolation for UKWA medians
</commit_message>
<xml_diff>
--- a/resources/ukwa/analysis/percentiles.xlsx
+++ b/resources/ukwa/analysis/percentiles.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wsw-results\resources\ukwa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wsw-results\resources\ukwa\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE58497B-54EF-4608-A6E1-D5B8F5A764F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ABC074-105F-4784-9FB0-D98B5D5D942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BC2B614C-97CE-4BFB-A796-CE0AF2755093}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>25th percentile</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Note this is an illustration which uses average speeds, not second best speed</t>
+  </si>
+  <si>
+    <t>50th percentile</t>
   </si>
 </sst>
 </file>
@@ -3968,10 +3971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF0D37A-FE3E-4993-BE94-996EF6CE4A41}">
-  <dimension ref="A1:K123"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4039,7 +4042,7 @@
         <v/>
       </c>
       <c r="I2" s="5" t="str">
-        <f t="shared" ref="I2:I33" si="3">IF(C2&gt;=28,"Y","")</f>
+        <f t="shared" ref="I2:I4" si="3">IF(C2&gt;=28,"Y","")</f>
         <v/>
       </c>
       <c r="J2" s="5" t="str">
@@ -6513,7 +6516,7 @@
         <v/>
       </c>
       <c r="J67" s="5" t="str">
-        <f t="shared" ref="J67:J118" si="11">IF(D67&gt;=26,"Y","")</f>
+        <f t="shared" ref="J67:J117" si="11">IF(D67&gt;=26,"Y","")</f>
         <v/>
       </c>
       <c r="K67" s="5" t="str">
@@ -6623,7 +6626,7 @@
         <v/>
       </c>
       <c r="I70" s="5" t="str">
-        <f t="shared" ref="I70:I118" si="13">IF(C70&gt;=28,"Y","")</f>
+        <f t="shared" ref="I70:I117" si="13">IF(C70&gt;=28,"Y","")</f>
         <v>Y</v>
       </c>
       <c r="J70" s="5" t="str">
@@ -8426,7 +8429,7 @@
         <v>115</v>
       </c>
       <c r="F118" s="4">
-        <f t="shared" ref="F118:J118" si="16">COUNT(F$2:F$117)</f>
+        <f t="shared" ref="F118:G118" si="16">COUNT(F$2:F$117)</f>
         <v>8</v>
       </c>
       <c r="G118" s="4">
@@ -8515,6 +8518,30 @@
       <c r="G123" s="1">
         <f>MAX(G$2:G$117)</f>
         <v>2.5800000000000018</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" s="1">
+        <v>28</v>
+      </c>
+      <c r="E125">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>13</v>
+      </c>
+      <c r="D126" s="2">
+        <f>FORECAST(D125,$D2:$D117,$C2:$C117)</f>
+        <v>26.076343588135487</v>
+      </c>
+      <c r="E126" s="2">
+        <f>FORECAST(E125,$D2:$D117,$C2:$C117)</f>
+        <v>24.236651472800713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor tweak to UKWA spreadsheet
</commit_message>
<xml_diff>
--- a/resources/ukwa/analysis/percentiles.xlsx
+++ b/resources/ukwa/analysis/percentiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wsw-results\resources\ukwa\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ABC074-105F-4784-9FB0-D98B5D5D942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A493C9B-3C59-4044-983D-E4AD41FBD219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BC2B614C-97CE-4BFB-A796-CE0AF2755093}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>25th percentile</t>
   </si>
@@ -79,11 +79,17 @@
   <si>
     <t>50th percentile</t>
   </si>
+  <si>
+    <t>persons</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -162,6 +168,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -286,11 +296,25 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$116</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="115"/>
                 <c:pt idx="0">
                   <c:v>24.59</c:v>
@@ -644,7 +668,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$116</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="115"/>
                 <c:pt idx="0">
                   <c:v>22.57</c:v>
@@ -1088,7 +1112,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1133,6 +1157,7 @@
         <c:axId val="1230299248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="35"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1205,7 +1230,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1407,11 +1432,25 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$116</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="115"/>
                 <c:pt idx="0">
                   <c:v>24.59</c:v>
@@ -1765,7 +1804,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$116</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="115"/>
                 <c:pt idx="0">
                   <c:v>22.57</c:v>
@@ -2137,8 +2176,8 @@
         <c:axId val="1231959152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="30"/>
-          <c:min val="24"/>
+          <c:max val="29"/>
+          <c:min val="27"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2211,7 +2250,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2257,8 +2296,8 @@
         <c:axId val="1230299248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="28"/>
-          <c:min val="22"/>
+          <c:max val="27"/>
+          <c:min val="25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2331,7 +2370,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2422,7 +2461,6 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -3619,61 +3657,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.08608</cdr:x>
-      <cdr:y>0.16162</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.97131</cdr:x>
-      <cdr:y>0.86644</cdr:y>
-    </cdr:to>
-    <cdr:cxnSp macro="">
-      <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="3" name="Straight Connector 2">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE65456D-D23F-9680-9643-B28BB35DD2EB}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvCxnSpPr/>
-      </cdr:nvCxnSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="571479" y="685800"/>
-          <a:ext cx="5876946" cy="2990841"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:solidFill>
-            <a:srgbClr val="00B050"/>
-          </a:solidFill>
-        </a:ln>
-      </cdr:spPr>
-      <cdr:style>
-        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </cdr:style>
-    </cdr:cxnSp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3971,16 +3954,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF0D37A-FE3E-4993-BE94-996EF6CE4A41}">
-  <dimension ref="A1:K126"/>
+  <dimension ref="A1:Q123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -3991,6 +3974,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -4023,21 +4009,21 @@
       <c r="B2">
         <v>18</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>24.59</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>22.57</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <f t="shared" ref="E2:E33" si="0">C2-D2</f>
         <v>2.0199999999999996</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F2" s="1" t="str">
         <f t="shared" ref="F2:F65" si="1">IF($C2&lt;29,IF($C2&gt;28,$E2,""),"")</f>
         <v/>
       </c>
-      <c r="G2" t="str">
+      <c r="G2" s="1" t="str">
         <f t="shared" ref="G2:G65" si="2">IF($C2&lt;27,IF($C2&gt;26,$E2,""),"")</f>
         <v/>
       </c>
@@ -4061,21 +4047,21 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>16.239999999999998</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>16.13</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <f t="shared" si="0"/>
         <v>0.10999999999999943</v>
       </c>
-      <c r="F3" t="str">
+      <c r="F3" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G3" t="str">
+      <c r="G3" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4099,21 +4085,21 @@
       <c r="B4">
         <v>21</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>25.4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>24.91</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>0.48999999999999844</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F4" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G4" t="str">
+      <c r="G4" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4137,21 +4123,21 @@
       <c r="B5">
         <v>32</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>28.93</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>27.04</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>1.8900000000000006</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <f t="shared" si="1"/>
         <v>1.8900000000000006</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4175,21 +4161,21 @@
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>21.71</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>19.55</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>2.16</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F6" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G6" t="str">
+      <c r="G6" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4213,21 +4199,21 @@
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>19.63</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>18.55</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>1.0799999999999983</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F7" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G7" t="str">
+      <c r="G7" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4251,21 +4237,21 @@
       <c r="B8">
         <v>23</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>24.31</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>23.24</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>1.0700000000000003</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F8" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G8" t="str">
+      <c r="G8" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4289,21 +4275,21 @@
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>10.66</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>9.01</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>1.6500000000000004</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F9" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G9" t="str">
+      <c r="G9" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4327,21 +4313,21 @@
       <c r="B10">
         <v>12</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>16.420000000000002</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>14.79</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>1.6300000000000026</v>
       </c>
-      <c r="F10" t="str">
+      <c r="F10" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G10" t="str">
+      <c r="G10" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4365,21 +4351,21 @@
       <c r="B11">
         <v>33</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>32.659999999999997</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>30.34</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <f t="shared" si="0"/>
         <v>2.3199999999999967</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F11" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G11" t="str">
+      <c r="G11" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4403,21 +4389,21 @@
       <c r="B12">
         <v>24</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>29.7</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>27.99</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>1.7100000000000009</v>
       </c>
-      <c r="F12" t="str">
+      <c r="F12" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G12" t="str">
+      <c r="G12" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4441,21 +4427,21 @@
       <c r="B13">
         <v>18</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>27.63</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>26.35</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <f t="shared" si="0"/>
         <v>1.2799999999999976</v>
       </c>
-      <c r="F13" t="str">
+      <c r="F13" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G13" t="str">
+      <c r="G13" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4479,21 +4465,21 @@
       <c r="B14">
         <v>19</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>23.49</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>22.69</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <f t="shared" si="0"/>
         <v>0.79999999999999716</v>
       </c>
-      <c r="F14" t="str">
+      <c r="F14" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G14" t="str">
+      <c r="G14" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4517,21 +4503,21 @@
       <c r="B15">
         <v>7</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>19.850000000000001</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>19.55</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <f t="shared" si="0"/>
         <v>0.30000000000000071</v>
       </c>
-      <c r="F15" t="str">
+      <c r="F15" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G15" t="str">
+      <c r="G15" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4555,21 +4541,21 @@
       <c r="B16">
         <v>5</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>21.81</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>20.05</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <f t="shared" si="0"/>
         <v>1.759999999999998</v>
       </c>
-      <c r="F16" t="str">
+      <c r="F16" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G16" t="str">
+      <c r="G16" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4593,21 +4579,21 @@
       <c r="B17">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>18.989999999999998</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>18.72</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>0.26999999999999957</v>
       </c>
-      <c r="F17" t="str">
+      <c r="F17" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G17" t="str">
+      <c r="G17" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4631,21 +4617,21 @@
       <c r="B18">
         <v>19</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>27.58</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>25.62</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <f t="shared" si="0"/>
         <v>1.9599999999999973</v>
       </c>
-      <c r="F18" t="str">
+      <c r="F18" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G18" t="str">
+      <c r="G18" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4669,21 +4655,21 @@
       <c r="B19">
         <v>19</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>26.84</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>24.81</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <f t="shared" si="0"/>
         <v>2.0300000000000011</v>
       </c>
-      <c r="F19" t="str">
+      <c r="F19" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <f t="shared" si="2"/>
         <v>2.0300000000000011</v>
       </c>
@@ -4707,21 +4693,21 @@
       <c r="B20">
         <v>13</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>28.08</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>25.6</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>2.4799999999999969</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <f t="shared" si="1"/>
         <v>2.4799999999999969</v>
       </c>
-      <c r="G20" t="str">
+      <c r="G20" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4745,21 +4731,21 @@
       <c r="B21">
         <v>18</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>28.65</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>26.13</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>2.5199999999999996</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <f t="shared" si="1"/>
         <v>2.5199999999999996</v>
       </c>
-      <c r="G21" t="str">
+      <c r="G21" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4783,21 +4769,21 @@
       <c r="B22">
         <v>6</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>21.66</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>19.45</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>2.2100000000000009</v>
       </c>
-      <c r="F22" t="str">
+      <c r="F22" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G22" t="str">
+      <c r="G22" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4821,21 +4807,21 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>22.96</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>22.96</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" t="str">
+      <c r="F23" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G23" t="str">
+      <c r="G23" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4859,21 +4845,21 @@
       <c r="B24">
         <v>24</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>29</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>27.15</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>1.8500000000000014</v>
       </c>
-      <c r="F24" t="str">
+      <c r="F24" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G24" t="str">
+      <c r="G24" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4897,21 +4883,21 @@
       <c r="B25">
         <v>27</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>26.15</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>24.14</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>2.009999999999998</v>
       </c>
-      <c r="F25" t="str">
+      <c r="F25" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <f t="shared" si="2"/>
         <v>2.009999999999998</v>
       </c>
@@ -4935,21 +4921,21 @@
       <c r="B26">
         <v>18</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>24.32</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>22.7</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <f t="shared" si="0"/>
         <v>1.620000000000001</v>
       </c>
-      <c r="F26" t="str">
+      <c r="F26" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G26" t="str">
+      <c r="G26" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4973,21 +4959,21 @@
       <c r="B27">
         <v>14</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>20.39</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>18.54</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <f t="shared" si="0"/>
         <v>1.8500000000000014</v>
       </c>
-      <c r="F27" t="str">
+      <c r="F27" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G27" t="str">
+      <c r="G27" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5011,21 +4997,21 @@
       <c r="B28">
         <v>18</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>27.47</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>26.39</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <f t="shared" si="0"/>
         <v>1.0799999999999983</v>
       </c>
-      <c r="F28" t="str">
+      <c r="F28" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G28" t="str">
+      <c r="G28" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5049,21 +5035,21 @@
       <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>30.14</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>28.94</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <f t="shared" si="0"/>
         <v>1.1999999999999993</v>
       </c>
-      <c r="F29" t="str">
+      <c r="F29" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G29" t="str">
+      <c r="G29" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5087,21 +5073,21 @@
       <c r="B30">
         <v>27</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>26.14</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>24.57</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <f t="shared" si="0"/>
         <v>1.5700000000000003</v>
       </c>
-      <c r="F30" t="str">
+      <c r="F30" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <f t="shared" si="2"/>
         <v>1.5700000000000003</v>
       </c>
@@ -5125,21 +5111,21 @@
       <c r="B31">
         <v>10</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>29.85</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>28.28</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <f t="shared" si="0"/>
         <v>1.5700000000000003</v>
       </c>
-      <c r="F31" t="str">
+      <c r="F31" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G31" t="str">
+      <c r="G31" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5163,21 +5149,21 @@
       <c r="B32">
         <v>15</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>27.71</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>25.44</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <f t="shared" si="0"/>
         <v>2.2699999999999996</v>
       </c>
-      <c r="F32" t="str">
+      <c r="F32" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G32" t="str">
+      <c r="G32" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5194,28 +5180,28 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20141018</v>
       </c>
       <c r="B33">
         <v>19</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>27.3</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>25.36</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <f t="shared" si="0"/>
         <v>1.9400000000000013</v>
       </c>
-      <c r="F33" t="str">
+      <c r="F33" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G33" t="str">
+      <c r="G33" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5232,28 +5218,28 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20141019</v>
       </c>
       <c r="B34">
         <v>24</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>31.1</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>28.98</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <f t="shared" ref="E34:E65" si="7">C34-D34</f>
         <v>2.120000000000001</v>
       </c>
-      <c r="F34" t="str">
+      <c r="F34" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G34" t="str">
+      <c r="G34" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5270,28 +5256,28 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20141019</v>
       </c>
       <c r="B35">
         <v>22</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>30.39</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>28.28</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <f t="shared" si="7"/>
         <v>2.1099999999999994</v>
       </c>
-      <c r="F35" t="str">
+      <c r="F35" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G35" t="str">
+      <c r="G35" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5308,28 +5294,28 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>20141020</v>
       </c>
       <c r="B36">
         <v>15</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>30.42</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>29.24</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <f t="shared" si="7"/>
         <v>1.1800000000000033</v>
       </c>
-      <c r="F36" t="str">
+      <c r="F36" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G36" t="str">
+      <c r="G36" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5346,28 +5332,28 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>20141020</v>
       </c>
       <c r="B37">
         <v>15</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>30.99</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>28.93</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <f t="shared" si="7"/>
         <v>2.0599999999999987</v>
       </c>
-      <c r="F37" t="str">
+      <c r="F37" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G37" t="str">
+      <c r="G37" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5384,28 +5370,28 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>20141021</v>
       </c>
       <c r="B38">
         <v>14</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>31.77</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>29.54</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <f t="shared" si="7"/>
         <v>2.2300000000000004</v>
       </c>
-      <c r="F38" t="str">
+      <c r="F38" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G38" t="str">
+      <c r="G38" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5422,28 +5408,28 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>20141021</v>
       </c>
       <c r="B39">
         <v>14</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>30.16</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>27.61</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <f t="shared" si="7"/>
         <v>2.5500000000000007</v>
       </c>
-      <c r="F39" t="str">
+      <c r="F39" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G39" t="str">
+      <c r="G39" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5460,28 +5446,28 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>20141022</v>
       </c>
       <c r="B40">
         <v>15</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>25.27</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>24.43</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <f t="shared" si="7"/>
         <v>0.83999999999999986</v>
       </c>
-      <c r="F40" t="str">
+      <c r="F40" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G40" t="str">
+      <c r="G40" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5498,28 +5484,28 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>20141022</v>
       </c>
       <c r="B41">
         <v>6</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>22.12</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>21.97</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <f t="shared" si="7"/>
         <v>0.15000000000000213</v>
       </c>
-      <c r="F41" t="str">
+      <c r="F41" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G41" t="str">
+      <c r="G41" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5536,28 +5522,28 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>20141023</v>
       </c>
       <c r="B42">
         <v>19</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>30.87</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>28.59</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <f t="shared" si="7"/>
         <v>2.2800000000000011</v>
       </c>
-      <c r="F42" t="str">
+      <c r="F42" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G42" t="str">
+      <c r="G42" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5574,28 +5560,28 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>20141023</v>
       </c>
       <c r="B43">
         <v>18</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>28.96</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>27.56</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="1">
         <f t="shared" si="7"/>
         <v>1.4000000000000021</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <f t="shared" si="1"/>
         <v>1.4000000000000021</v>
       </c>
-      <c r="G43" t="str">
+      <c r="G43" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5612,28 +5598,28 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>20151003</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>3.67</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>3.67</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F44" t="str">
+      <c r="F44" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G44" t="str">
+      <c r="G44" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5650,28 +5636,28 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>20151004</v>
       </c>
       <c r="B45">
         <v>21</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>25.91</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>25.62</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="1">
         <f t="shared" si="7"/>
         <v>0.28999999999999915</v>
       </c>
-      <c r="F45" t="str">
+      <c r="F45" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G45" t="str">
+      <c r="G45" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5688,28 +5674,28 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>20151004</v>
       </c>
       <c r="B46">
         <v>10</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <v>24.46</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>22.48</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="1">
         <f t="shared" si="7"/>
         <v>1.9800000000000004</v>
       </c>
-      <c r="F46" t="str">
+      <c r="F46" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G46" t="str">
+      <c r="G46" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5726,28 +5712,28 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>20151005</v>
       </c>
       <c r="B47">
         <v>25</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>28.62</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>26.35</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="1">
         <f t="shared" si="7"/>
         <v>2.2699999999999996</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="1">
         <f t="shared" si="1"/>
         <v>2.2699999999999996</v>
       </c>
-      <c r="G47" t="str">
+      <c r="G47" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5764,28 +5750,28 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20151005</v>
       </c>
       <c r="B48">
         <v>24</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <v>27.53</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>26.21</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="1">
         <f t="shared" si="7"/>
         <v>1.3200000000000003</v>
       </c>
-      <c r="F48" t="str">
+      <c r="F48" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G48" t="str">
+      <c r="G48" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5801,29 +5787,38 @@
         <f t="shared" si="5"/>
         <v>Y</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>0</v>
+      </c>
+      <c r="P48" s="1">
+        <v>28</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>20151006</v>
       </c>
       <c r="B49">
         <v>4</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>20.95</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>20.07</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="1">
         <f t="shared" si="7"/>
         <v>0.87999999999999901</v>
       </c>
-      <c r="F49" t="str">
+      <c r="F49" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G49" t="str">
+      <c r="G49" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5839,29 +5834,40 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
+        <v>13</v>
+      </c>
+      <c r="P49" s="2">
+        <f>FORECAST(P48,$D2:$D117,$C2:$C117)</f>
+        <v>26.076343588135487</v>
+      </c>
+      <c r="Q49" s="2">
+        <f>FORECAST(Q48,$D2:$D117,$C2:$C117)</f>
+        <v>24.236651472800713</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>20151006</v>
       </c>
       <c r="B50">
         <v>24</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <v>24.93</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>23.5</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="1">
         <f t="shared" si="7"/>
         <v>1.4299999999999997</v>
       </c>
-      <c r="F50" t="str">
+      <c r="F50" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G50" t="str">
+      <c r="G50" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5878,28 +5884,28 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>20151007</v>
       </c>
       <c r="B51">
         <v>10</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
         <v>29.81</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
         <v>26.7</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="1">
         <f t="shared" si="7"/>
         <v>3.1099999999999994</v>
       </c>
-      <c r="F51" t="str">
+      <c r="F51" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G51" t="str">
+      <c r="G51" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5916,28 +5922,28 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>20151007</v>
       </c>
       <c r="B52">
         <v>26</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
         <v>29.88</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
         <v>28.97</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="1">
         <f t="shared" si="7"/>
         <v>0.91000000000000014</v>
       </c>
-      <c r="F52" t="str">
+      <c r="F52" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G52" t="str">
+      <c r="G52" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5954,28 +5960,28 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>20161008</v>
       </c>
       <c r="B53">
         <v>7</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="1">
         <v>20.100000000000001</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="1">
         <v>19.12</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="1">
         <f t="shared" si="7"/>
         <v>0.98000000000000043</v>
       </c>
-      <c r="F53" t="str">
+      <c r="F53" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G53" t="str">
+      <c r="G53" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5992,28 +5998,28 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>20161009</v>
       </c>
       <c r="B54">
         <v>8</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="1">
         <v>20.34</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="1">
         <v>17.97</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="1">
         <f t="shared" si="7"/>
         <v>2.370000000000001</v>
       </c>
-      <c r="F54" t="str">
+      <c r="F54" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G54" t="str">
+      <c r="G54" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6030,28 +6036,28 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>20161009</v>
       </c>
       <c r="B55">
         <v>13</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="1">
         <v>22</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="1">
         <v>19.77</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="1">
         <f t="shared" si="7"/>
         <v>2.2300000000000004</v>
       </c>
-      <c r="F55" t="str">
+      <c r="F55" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G55" t="str">
+      <c r="G55" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6068,28 +6074,28 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20161010</v>
       </c>
       <c r="B56">
         <v>6</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="1">
         <v>18.47</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="1">
         <v>18.04</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="1">
         <f t="shared" si="7"/>
         <v>0.42999999999999972</v>
       </c>
-      <c r="F56" t="str">
+      <c r="F56" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G56" t="str">
+      <c r="G56" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6106,28 +6112,28 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>20161011</v>
       </c>
       <c r="B57">
         <v>16</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="1">
         <v>25.23</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="1">
         <v>22.82</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="1">
         <f t="shared" si="7"/>
         <v>2.41</v>
       </c>
-      <c r="F57" t="str">
+      <c r="F57" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G57" t="str">
+      <c r="G57" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6144,28 +6150,28 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>20161011</v>
       </c>
       <c r="B58">
         <v>13</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="1">
         <v>25.59</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="1">
         <v>23.5</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="1">
         <f t="shared" si="7"/>
         <v>2.09</v>
       </c>
-      <c r="F58" t="str">
+      <c r="F58" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G58" t="str">
+      <c r="G58" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6182,28 +6188,28 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>20161012</v>
       </c>
       <c r="B59">
         <v>23</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="1">
         <v>27.78</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="1">
         <v>25.58</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="1">
         <f t="shared" si="7"/>
         <v>2.2000000000000028</v>
       </c>
-      <c r="F59" t="str">
+      <c r="F59" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G59" t="str">
+      <c r="G59" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6220,28 +6226,28 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>20161012</v>
       </c>
       <c r="B60">
         <v>23</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="1">
         <v>26.87</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="1">
         <v>24.41</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="1">
         <f t="shared" si="7"/>
         <v>2.4600000000000009</v>
       </c>
-      <c r="F60" t="str">
+      <c r="F60" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G60">
+      <c r="G60" s="1">
         <f t="shared" si="2"/>
         <v>2.4600000000000009</v>
       </c>
@@ -6258,28 +6264,28 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>20161013</v>
       </c>
       <c r="B61">
         <v>12</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="1">
         <v>27.2</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="1">
         <v>23.88</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="1">
         <f t="shared" si="7"/>
         <v>3.3200000000000003</v>
       </c>
-      <c r="F61" t="str">
+      <c r="F61" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G61" t="str">
+      <c r="G61" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6296,28 +6302,28 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>20161013</v>
       </c>
       <c r="B62">
         <v>24</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="1">
         <v>28.49</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="1">
         <v>26.7</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="1">
         <f t="shared" si="7"/>
         <v>1.7899999999999991</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="1">
         <f t="shared" si="1"/>
         <v>1.7899999999999991</v>
       </c>
-      <c r="G62" t="str">
+      <c r="G62" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6334,28 +6340,28 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>20161014</v>
       </c>
       <c r="B63">
         <v>9</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="1">
         <v>25.16</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="1">
         <v>24.01</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="1">
         <f t="shared" si="7"/>
         <v>1.1499999999999986</v>
       </c>
-      <c r="F63" t="str">
+      <c r="F63" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G63" t="str">
+      <c r="G63" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6372,28 +6378,28 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>20171015</v>
       </c>
       <c r="B64">
         <v>19</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="1">
         <v>25.41</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="1">
         <v>23.35</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="1">
         <f t="shared" si="7"/>
         <v>2.0599999999999987</v>
       </c>
-      <c r="F64" t="str">
+      <c r="F64" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G64" t="str">
+      <c r="G64" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6417,21 +6423,21 @@
       <c r="B65">
         <v>23</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="1">
         <v>34.25</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="1">
         <v>33.25</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="1">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="F65" t="str">
+      <c r="F65" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G65" t="str">
+      <c r="G65" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6455,21 +6461,21 @@
       <c r="B66">
         <v>21</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="1">
         <v>33.68</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="1">
         <v>30.94</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="1">
         <f t="shared" ref="E66:E97" si="8">C66-D66</f>
         <v>2.7399999999999984</v>
       </c>
-      <c r="F66" t="str">
+      <c r="F66" s="1" t="str">
         <f t="shared" ref="F66:F116" si="9">IF($C66&lt;29,IF($C66&gt;28,$E66,""),"")</f>
         <v/>
       </c>
-      <c r="G66" t="str">
+      <c r="G66" s="1" t="str">
         <f t="shared" ref="G66:G116" si="10">IF($C66&lt;27,IF($C66&gt;26,$E66,""),"")</f>
         <v/>
       </c>
@@ -6493,21 +6499,21 @@
       <c r="B67">
         <v>7</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="1">
         <v>20.98</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="1">
         <v>19.38</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="1">
         <f t="shared" si="8"/>
         <v>1.6000000000000014</v>
       </c>
-      <c r="F67" t="str">
+      <c r="F67" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G67" t="str">
+      <c r="G67" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6531,21 +6537,21 @@
       <c r="B68">
         <v>17</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="1">
         <v>28.66</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="1">
         <v>26.73</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="1">
         <f t="shared" si="8"/>
         <v>1.9299999999999997</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="1">
         <f t="shared" si="9"/>
         <v>1.9299999999999997</v>
       </c>
-      <c r="G68" t="str">
+      <c r="G68" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6569,21 +6575,21 @@
       <c r="B69">
         <v>2</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="1">
         <v>21.99</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="1">
         <v>21.99</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F69" t="str">
+      <c r="F69" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G69" t="str">
+      <c r="G69" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6607,21 +6613,21 @@
       <c r="B70">
         <v>15</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="1">
         <v>34.22</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="1">
         <v>30.81</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="1">
         <f t="shared" si="8"/>
         <v>3.41</v>
       </c>
-      <c r="F70" t="str">
+      <c r="F70" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G70" t="str">
+      <c r="G70" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6645,21 +6651,21 @@
       <c r="B71">
         <v>25</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="1">
         <v>30.08</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="1">
         <v>27.87</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="1">
         <f t="shared" si="8"/>
         <v>2.2099999999999973</v>
       </c>
-      <c r="F71" t="str">
+      <c r="F71" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G71" t="str">
+      <c r="G71" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6683,21 +6689,21 @@
       <c r="B72">
         <v>25</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="1">
         <v>29.25</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="1">
         <v>26.11</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="1">
         <f t="shared" si="8"/>
         <v>3.1400000000000006</v>
       </c>
-      <c r="F72" t="str">
+      <c r="F72" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G72" t="str">
+      <c r="G72" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6721,21 +6727,21 @@
       <c r="B73">
         <v>18</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="1">
         <v>30.25</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="1">
         <v>28.12</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="1">
         <f t="shared" si="8"/>
         <v>2.129999999999999</v>
       </c>
-      <c r="F73" t="str">
+      <c r="F73" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G73" t="str">
+      <c r="G73" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6759,21 +6765,21 @@
       <c r="B74">
         <v>9</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="1">
         <v>25.58</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="1">
         <v>24.05</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="1">
         <f t="shared" si="8"/>
         <v>1.5299999999999976</v>
       </c>
-      <c r="F74" t="str">
+      <c r="F74" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G74" t="str">
+      <c r="G74" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6797,21 +6803,21 @@
       <c r="B75">
         <v>18</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="1">
         <v>30.38</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="1">
         <v>28.83</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="1">
         <f t="shared" si="8"/>
         <v>1.5500000000000007</v>
       </c>
-      <c r="F75" t="str">
+      <c r="F75" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G75" t="str">
+      <c r="G75" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6835,21 +6841,21 @@
       <c r="B76">
         <v>22</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="1">
         <v>26.34</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="1">
         <v>24.17</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="1">
         <f t="shared" si="8"/>
         <v>2.1699999999999982</v>
       </c>
-      <c r="F76" t="str">
+      <c r="F76" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G76">
+      <c r="G76" s="1">
         <f t="shared" si="10"/>
         <v>2.1699999999999982</v>
       </c>
@@ -6873,21 +6879,21 @@
       <c r="B77">
         <v>1</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="1">
         <v>13.06</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="1">
         <v>13.06</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F77" t="str">
+      <c r="F77" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G77" t="str">
+      <c r="G77" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6911,21 +6917,21 @@
       <c r="B78">
         <v>6</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="1">
         <v>23.68</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="1">
         <v>22.28</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="1">
         <f t="shared" si="8"/>
         <v>1.3999999999999986</v>
       </c>
-      <c r="F78" t="str">
+      <c r="F78" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G78" t="str">
+      <c r="G78" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6949,21 +6955,21 @@
       <c r="B79">
         <v>19</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="1">
         <v>28.62</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="1">
         <v>26.1</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="1">
         <f t="shared" si="8"/>
         <v>2.5199999999999996</v>
       </c>
-      <c r="F79">
+      <c r="F79" s="1">
         <f t="shared" si="9"/>
         <v>2.5199999999999996</v>
       </c>
-      <c r="G79" t="str">
+      <c r="G79" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -6987,21 +6993,21 @@
       <c r="B80">
         <v>3</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="1">
         <v>19.61</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="1">
         <v>17.579999999999998</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="1">
         <f t="shared" si="8"/>
         <v>2.0300000000000011</v>
       </c>
-      <c r="F80" t="str">
+      <c r="F80" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G80" t="str">
+      <c r="G80" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7025,21 +7031,21 @@
       <c r="B81">
         <v>18</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="1">
         <v>31.2</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="1">
         <v>29.98</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="1">
         <f t="shared" si="8"/>
         <v>1.2199999999999989</v>
       </c>
-      <c r="F81" t="str">
+      <c r="F81" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G81" t="str">
+      <c r="G81" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7063,21 +7069,21 @@
       <c r="B82">
         <v>19</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="1">
         <v>30.52</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="1">
         <v>29</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="1">
         <f t="shared" si="8"/>
         <v>1.5199999999999996</v>
       </c>
-      <c r="F82" t="str">
+      <c r="F82" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G82" t="str">
+      <c r="G82" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7101,21 +7107,21 @@
       <c r="B83">
         <v>9</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="1">
         <v>33.99</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="1">
         <v>31.64</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="1">
         <f t="shared" si="8"/>
         <v>2.3500000000000014</v>
       </c>
-      <c r="F83" t="str">
+      <c r="F83" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G83" t="str">
+      <c r="G83" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7139,21 +7145,21 @@
       <c r="B84">
         <v>9</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="1">
         <v>33.549999999999997</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="1">
         <v>31.82</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="1">
         <f t="shared" si="8"/>
         <v>1.7299999999999969</v>
       </c>
-      <c r="F84" t="str">
+      <c r="F84" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G84" t="str">
+      <c r="G84" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7177,21 +7183,21 @@
       <c r="B85">
         <v>20</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="1">
         <v>32.21</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="1">
         <v>30.18</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="1">
         <f t="shared" si="8"/>
         <v>2.0300000000000011</v>
       </c>
-      <c r="F85" t="str">
+      <c r="F85" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G85" t="str">
+      <c r="G85" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7215,21 +7221,21 @@
       <c r="B86">
         <v>19</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="1">
         <v>31.44</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="1">
         <v>29.46</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="1">
         <f t="shared" si="8"/>
         <v>1.9800000000000004</v>
       </c>
-      <c r="F86" t="str">
+      <c r="F86" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G86" t="str">
+      <c r="G86" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7253,21 +7259,21 @@
       <c r="B87">
         <v>19</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="1">
         <v>30.89</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="1">
         <v>29.25</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="1">
         <f t="shared" si="8"/>
         <v>1.6400000000000006</v>
       </c>
-      <c r="F87" t="str">
+      <c r="F87" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G87" t="str">
+      <c r="G87" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7291,21 +7297,21 @@
       <c r="B88">
         <v>11</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="1">
         <v>32.76</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="1">
         <v>31.74</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="1">
         <f t="shared" si="8"/>
         <v>1.0199999999999996</v>
       </c>
-      <c r="F88" t="str">
+      <c r="F88" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G88" t="str">
+      <c r="G88" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7329,21 +7335,21 @@
       <c r="B89">
         <v>18</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="1">
         <v>31.82</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="1">
         <v>30.5</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="1">
         <f t="shared" si="8"/>
         <v>1.3200000000000003</v>
       </c>
-      <c r="F89" t="str">
+      <c r="F89" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G89" t="str">
+      <c r="G89" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7367,21 +7373,21 @@
       <c r="B90">
         <v>12</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="1">
         <v>32.619999999999997</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="1">
         <v>29.86</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="1">
         <f t="shared" si="8"/>
         <v>2.759999999999998</v>
       </c>
-      <c r="F90" t="str">
+      <c r="F90" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G90" t="str">
+      <c r="G90" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7405,21 +7411,21 @@
       <c r="B91">
         <v>16</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="1">
         <v>36.39</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="1">
         <v>33.46</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="1">
         <f t="shared" si="8"/>
         <v>2.9299999999999997</v>
       </c>
-      <c r="F91" t="str">
+      <c r="F91" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G91" t="str">
+      <c r="G91" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7443,21 +7449,21 @@
       <c r="B92">
         <v>17</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="1">
         <v>35.47</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="1">
         <v>32.950000000000003</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="1">
         <f t="shared" si="8"/>
         <v>2.519999999999996</v>
       </c>
-      <c r="F92" t="str">
+      <c r="F92" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G92" t="str">
+      <c r="G92" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7481,21 +7487,21 @@
       <c r="B93">
         <v>6</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="1">
         <v>23.81</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="1">
         <v>21.35</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="1">
         <f t="shared" si="8"/>
         <v>2.4599999999999973</v>
       </c>
-      <c r="F93" t="str">
+      <c r="F93" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G93" t="str">
+      <c r="G93" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7519,21 +7525,21 @@
       <c r="B94">
         <v>3</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="1">
         <v>21.88</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="1">
         <v>20.170000000000002</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="1">
         <f t="shared" si="8"/>
         <v>1.7099999999999973</v>
       </c>
-      <c r="F94" t="str">
+      <c r="F94" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G94" t="str">
+      <c r="G94" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7557,21 +7563,21 @@
       <c r="B95">
         <v>8</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="1">
         <v>23.62</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="1">
         <v>19.87</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="1">
         <f t="shared" si="8"/>
         <v>3.75</v>
       </c>
-      <c r="F95" t="str">
+      <c r="F95" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G95" t="str">
+      <c r="G95" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7595,21 +7601,21 @@
       <c r="B96">
         <v>3</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="1">
         <v>20.77</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="1">
         <v>18.77</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="1">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="F96" t="str">
+      <c r="F96" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G96" t="str">
+      <c r="G96" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7633,21 +7639,21 @@
       <c r="B97">
         <v>9</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="1">
         <v>22.82</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="1">
         <v>18.25</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="1">
         <f t="shared" si="8"/>
         <v>4.57</v>
       </c>
-      <c r="F97" t="str">
+      <c r="F97" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G97" t="str">
+      <c r="G97" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7671,21 +7677,21 @@
       <c r="B98">
         <v>31</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="1">
         <v>30.22</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="1">
         <v>26.94</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="1">
         <f t="shared" ref="E98:E108" si="14">C98-D98</f>
         <v>3.2799999999999976</v>
       </c>
-      <c r="F98" t="str">
+      <c r="F98" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G98" t="str">
+      <c r="G98" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7709,21 +7715,21 @@
       <c r="B99">
         <v>34</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="1">
         <v>31.98</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="1">
         <v>29.89</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="1">
         <f t="shared" si="14"/>
         <v>2.09</v>
       </c>
-      <c r="F99" t="str">
+      <c r="F99" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G99" t="str">
+      <c r="G99" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7747,21 +7753,21 @@
       <c r="B100">
         <v>11</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="1">
         <v>26.84</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="1">
         <v>24.91</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="1">
         <f t="shared" si="14"/>
         <v>1.9299999999999997</v>
       </c>
-      <c r="F100" t="str">
+      <c r="F100" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G100">
+      <c r="G100" s="1">
         <f t="shared" si="10"/>
         <v>1.9299999999999997</v>
       </c>
@@ -7785,21 +7791,21 @@
       <c r="B101">
         <v>21</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="1">
         <v>25.77</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="1">
         <v>24.63</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="1">
         <f t="shared" si="14"/>
         <v>1.1400000000000006</v>
       </c>
-      <c r="F101" t="str">
+      <c r="F101" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G101" t="str">
+      <c r="G101" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7823,21 +7829,21 @@
       <c r="B102">
         <v>5</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="1">
         <v>23.17</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="1">
         <v>22.76</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="1">
         <f t="shared" si="14"/>
         <v>0.41000000000000014</v>
       </c>
-      <c r="F102" t="str">
+      <c r="F102" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G102" t="str">
+      <c r="G102" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7861,21 +7867,21 @@
       <c r="B103">
         <v>22</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="1">
         <v>27.73</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="1">
         <v>26.1</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="1">
         <f t="shared" si="14"/>
         <v>1.629999999999999</v>
       </c>
-      <c r="F103" t="str">
+      <c r="F103" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G103" t="str">
+      <c r="G103" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7899,21 +7905,21 @@
       <c r="B104">
         <v>11</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="1">
         <v>30.55</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="1">
         <v>24.05</v>
       </c>
-      <c r="E104">
+      <c r="E104" s="1">
         <f t="shared" si="14"/>
         <v>6.5</v>
       </c>
-      <c r="F104" t="str">
+      <c r="F104" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G104" t="str">
+      <c r="G104" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7937,21 +7943,21 @@
       <c r="B105">
         <v>12</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="1">
         <v>29.85</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="1">
         <v>26.64</v>
       </c>
-      <c r="E105">
+      <c r="E105" s="1">
         <f t="shared" si="14"/>
         <v>3.2100000000000009</v>
       </c>
-      <c r="F105" t="str">
+      <c r="F105" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G105" t="str">
+      <c r="G105" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -7975,21 +7981,21 @@
       <c r="B106">
         <v>8</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="1">
         <v>31.19</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="1">
         <v>27.46</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="1">
         <f t="shared" si="14"/>
         <v>3.7300000000000004</v>
       </c>
-      <c r="F106" t="str">
+      <c r="F106" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G106" t="str">
+      <c r="G106" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -8013,21 +8019,21 @@
       <c r="B107">
         <v>12</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="1">
         <v>31.9</v>
       </c>
-      <c r="D107">
+      <c r="D107" s="1">
         <v>28.89</v>
       </c>
-      <c r="E107">
+      <c r="E107" s="1">
         <f t="shared" si="14"/>
         <v>3.009999999999998</v>
       </c>
-      <c r="F107" t="str">
+      <c r="F107" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G107" t="str">
+      <c r="G107" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -8051,21 +8057,21 @@
       <c r="B108">
         <v>17</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="1">
         <v>22.8</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="1">
         <v>21.88</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="1">
         <f t="shared" si="14"/>
         <v>0.92000000000000171</v>
       </c>
-      <c r="F108" t="str">
+      <c r="F108" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G108" t="str">
+      <c r="G108" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -8089,17 +8095,21 @@
       <c r="B109">
         <v>12</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="1">
         <v>23.22</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="1">
         <v>22.05</v>
       </c>
-      <c r="F109" t="str">
+      <c r="E109" s="1">
+        <f t="shared" ref="E109:E117" si="15">C109-D109</f>
+        <v>1.1699999999999982</v>
+      </c>
+      <c r="F109" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G109" t="str">
+      <c r="G109" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -8123,21 +8133,21 @@
       <c r="B110">
         <v>14</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="1">
         <v>25.01</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="1">
         <v>24.15</v>
       </c>
-      <c r="E110">
-        <f t="shared" ref="E110:E117" si="15">C110-D110</f>
+      <c r="E110" s="1">
+        <f t="shared" si="15"/>
         <v>0.86000000000000298</v>
       </c>
-      <c r="F110" t="str">
+      <c r="F110" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G110" t="str">
+      <c r="G110" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -8161,21 +8171,21 @@
       <c r="B111">
         <v>13</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="1">
         <v>23.88</v>
       </c>
-      <c r="D111">
+      <c r="D111" s="1">
         <v>22.61</v>
       </c>
-      <c r="E111">
+      <c r="E111" s="1">
         <f t="shared" si="15"/>
         <v>1.2699999999999996</v>
       </c>
-      <c r="F111" t="str">
+      <c r="F111" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G111" t="str">
+      <c r="G111" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -8199,21 +8209,21 @@
       <c r="B112">
         <v>22</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="1">
         <v>26.72</v>
       </c>
-      <c r="D112">
+      <c r="D112" s="1">
         <v>25.66</v>
       </c>
-      <c r="E112">
+      <c r="E112" s="1">
         <f t="shared" si="15"/>
         <v>1.0599999999999987</v>
       </c>
-      <c r="F112" t="str">
+      <c r="F112" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G112">
+      <c r="G112" s="1">
         <f t="shared" si="10"/>
         <v>1.0599999999999987</v>
       </c>
@@ -8237,21 +8247,21 @@
       <c r="B113">
         <v>25</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="1">
         <v>27.6</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="1">
         <v>26.44</v>
       </c>
-      <c r="E113">
+      <c r="E113" s="1">
         <f t="shared" si="15"/>
         <v>1.1600000000000001</v>
       </c>
-      <c r="F113" t="str">
+      <c r="F113" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G113" t="str">
+      <c r="G113" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -8275,21 +8285,21 @@
       <c r="B114">
         <v>3</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="1">
         <v>26.69</v>
       </c>
-      <c r="D114">
+      <c r="D114" s="1">
         <v>24.11</v>
       </c>
-      <c r="E114">
+      <c r="E114" s="1">
         <f t="shared" si="15"/>
         <v>2.5800000000000018</v>
       </c>
-      <c r="F114" t="str">
+      <c r="F114" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G114">
+      <c r="G114" s="1">
         <f t="shared" si="10"/>
         <v>2.5800000000000018</v>
       </c>
@@ -8313,21 +8323,21 @@
       <c r="B115">
         <v>14</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="1">
         <v>29.08</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="1">
         <v>27.13</v>
       </c>
-      <c r="E115">
+      <c r="E115" s="1">
         <f t="shared" si="15"/>
         <v>1.9499999999999993</v>
       </c>
-      <c r="F115" t="str">
+      <c r="F115" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G115" t="str">
+      <c r="G115" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -8351,21 +8361,21 @@
       <c r="B116">
         <v>28</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="1">
         <v>31.08</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="1">
         <v>29.74</v>
       </c>
-      <c r="E116">
+      <c r="E116" s="1">
         <f t="shared" si="15"/>
         <v>1.3399999999999999</v>
       </c>
-      <c r="F116" t="str">
+      <c r="F116" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G116" t="str">
+      <c r="G116" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
@@ -8389,21 +8399,21 @@
       <c r="B117">
         <v>28</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="1">
         <v>32.39</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="1">
         <v>30.06</v>
       </c>
-      <c r="E117">
+      <c r="E117" s="1">
         <f t="shared" si="15"/>
         <v>2.3300000000000018</v>
       </c>
-      <c r="F117" t="str">
+      <c r="F117" s="1" t="str">
         <f>IF($C117&lt;29,IF($C117&gt;28,$E117,""),"")</f>
         <v/>
       </c>
-      <c r="G117" t="str">
+      <c r="G117" s="1" t="str">
         <f>IF($C117&lt;27,IF($C117&gt;26,$E117,""),"")</f>
         <v/>
       </c>
@@ -8426,7 +8436,7 @@
       </c>
       <c r="E118" s="4">
         <f>COUNT(E$2:E$117)</f>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F118" s="4">
         <f t="shared" ref="F118:G118" si="16">COUNT(F$2:F$117)</f>
@@ -8450,18 +8460,22 @@
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C120" t="s">
+      <c r="A120" t="s">
         <v>4</v>
+      </c>
+      <c r="B120" s="11">
+        <f>MIN(B$2:B$117)</f>
+        <v>1</v>
       </c>
       <c r="E120" s="3">
         <f>MIN(E$2:E$117)</f>
         <v>0</v>
       </c>
-      <c r="F120" s="1">
+      <c r="F120" s="9">
         <f>MIN(F$2:F$117)</f>
         <v>1.4000000000000021</v>
       </c>
-      <c r="G120" s="1">
+      <c r="G120" s="9">
         <f>MIN(G$2:G$117)</f>
         <v>1.0599999999999987</v>
       </c>
@@ -8470,78 +8484,66 @@
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C121" t="s">
+      <c r="A121" t="s">
         <v>1</v>
+      </c>
+      <c r="B121" s="12">
+        <f>MEDIAN(B$2:B$117)</f>
+        <v>15.5</v>
       </c>
       <c r="E121" s="3">
         <f>MEDIAN(E$2:E$117)</f>
-        <v>1.8900000000000006</v>
-      </c>
-      <c r="F121" s="2">
+        <v>1.870000000000001</v>
+      </c>
+      <c r="F121" s="10">
         <f>MEDIAN(F$2:F$117)</f>
         <v>2.0999999999999996</v>
       </c>
-      <c r="G121" s="2">
+      <c r="G121" s="10">
         <f>MEDIAN(G$2:G$117)</f>
         <v>2.0199999999999996</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C122" t="s">
+      <c r="A122" t="s">
         <v>3</v>
+      </c>
+      <c r="B122" s="12">
+        <f>AVERAGE(B$2:B$117)</f>
+        <v>15.379310344827585</v>
       </c>
       <c r="E122" s="3">
         <f>AVERAGE(E$2:E$117)</f>
-        <v>1.8136521739130436</v>
-      </c>
-      <c r="F122" s="2">
+        <v>1.8081034482758622</v>
+      </c>
+      <c r="F122" s="10">
         <f>AVERAGE(F$2:F$117)</f>
         <v>2.0999999999999996</v>
       </c>
-      <c r="G122" s="2">
+      <c r="G122" s="10">
         <f>AVERAGE(G$2:G$117)</f>
         <v>1.9762499999999998</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C123" t="s">
+      <c r="A123" t="s">
         <v>5</v>
+      </c>
+      <c r="B123" s="11">
+        <f>MAX(B$2:B$117)</f>
+        <v>34</v>
       </c>
       <c r="E123" s="3">
         <f>MAX(E$2:E$117)</f>
         <v>6.5</v>
       </c>
-      <c r="F123" s="1">
+      <c r="F123" s="9">
         <f>MAX(F$2:F$117)</f>
         <v>2.5199999999999996</v>
       </c>
-      <c r="G123" s="1">
+      <c r="G123" s="9">
         <f>MAX(G$2:G$117)</f>
         <v>2.5800000000000018</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C125" t="s">
-        <v>0</v>
-      </c>
-      <c r="D125" s="1">
-        <v>28</v>
-      </c>
-      <c r="E125">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C126" t="s">
-        <v>13</v>
-      </c>
-      <c r="D126" s="2">
-        <f>FORECAST(D125,$D2:$D117,$C2:$C117)</f>
-        <v>26.076343588135487</v>
-      </c>
-      <c r="E126" s="2">
-        <f>FORECAST(E125,$D2:$D117,$C2:$C117)</f>
-        <v>24.236651472800713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Perform further UKWA analysis using more approaches
</commit_message>
<xml_diff>
--- a/resources/ukwa/analysis/percentiles.xlsx
+++ b/resources/ukwa/analysis/percentiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wsw-results\resources\ukwa\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB910AE-2035-459C-A137-6F47EAFC697C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3AF855-EF60-4D54-955E-1CE60877740C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BC2B614C-97CE-4BFB-A796-CE0AF2755093}"/>
   </bookViews>
@@ -240,7 +240,7 @@
             </a:br>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>50th percentile (median) vs 25th percentile</a:t>
+              <a:t>50th percentile vs 25th percentile</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5528,8 +5528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF0D37A-FE3E-4993-BE94-996EF6CE4A41}">
   <dimension ref="A1:Y124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="T49" sqref="T49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7818,35 +7818,35 @@
         <v>13</v>
       </c>
       <c r="R49" s="2">
-        <f>FORECAST(R48,$D2:$D117,$C2:$C117)</f>
+        <f t="shared" ref="R49:Y49" si="10">FORECAST(R48,$D2:$D117,$C2:$C117)</f>
         <v>26.076343588135487</v>
       </c>
       <c r="S49" s="2">
-        <f>FORECAST(S48,$D2:$D117,$C2:$C117)</f>
+        <f t="shared" si="10"/>
         <v>25.156497530468101</v>
       </c>
       <c r="T49" s="2">
-        <f>FORECAST(T48,$D2:$D117,$C2:$C117)</f>
+        <f t="shared" si="10"/>
         <v>24.236651472800713</v>
       </c>
       <c r="U49" s="2">
-        <f>FORECAST(U48,$D2:$D117,$C2:$C117)</f>
+        <f t="shared" si="10"/>
         <v>23.316805415133324</v>
       </c>
       <c r="V49" s="2">
-        <f>FORECAST(V48,$D2:$D117,$C2:$C117)</f>
+        <f t="shared" si="10"/>
         <v>22.396959357465938</v>
       </c>
       <c r="W49" s="2">
-        <f>FORECAST(W48,$D2:$D117,$C2:$C117)</f>
+        <f t="shared" si="10"/>
         <v>21.477113299798553</v>
       </c>
       <c r="X49" s="2">
-        <f>FORECAST(X48,$D2:$D117,$C2:$C117)</f>
+        <f t="shared" si="10"/>
         <v>20.557267242131164</v>
       </c>
       <c r="Y49" s="2">
-        <f>FORECAST(Y48,$D2:$D117,$C2:$C117)</f>
+        <f t="shared" si="10"/>
         <v>19.637421184463776</v>
       </c>
     </row>
@@ -8600,7 +8600,7 @@
         <v>30.94</v>
       </c>
       <c r="E66" s="1">
-        <f t="shared" ref="E66:E97" si="10">C66-D66</f>
+        <f t="shared" ref="E66:E97" si="11">C66-D66</f>
         <v>2.7399999999999984</v>
       </c>
       <c r="F66" s="1" t="str">
@@ -8646,23 +8646,23 @@
         <v>19.38</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.6000000000000014</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f t="shared" ref="F67:F117" si="11">IF($C67&lt;28,IF($C67&gt;27,C67-I67,""),"")</f>
+        <f t="shared" ref="F67:F117" si="12">IF($C67&lt;28,IF($C67&gt;27,C67-I67,""),"")</f>
         <v/>
       </c>
       <c r="G67" s="1" t="str">
-        <f t="shared" ref="G67:G117" si="12">IF($C67&lt;26,IF($C67&gt;25,C67-I67,""),"")</f>
+        <f t="shared" ref="G67:G117" si="13">IF($C67&lt;26,IF($C67&gt;25,C67-I67,""),"")</f>
         <v/>
       </c>
       <c r="I67" s="1">
-        <f t="shared" ref="I67:I117" si="13">FORECAST(C67,$D$2:$D$117,$C$2:$C$117)</f>
+        <f t="shared" ref="I67:I117" si="14">FORECAST(C67,$D$2:$D$117,$C$2:$C$117)</f>
         <v>19.619024263310429</v>
       </c>
       <c r="J67" s="1">
-        <f t="shared" ref="J67:J117" si="14">D67-I67</f>
+        <f t="shared" ref="J67:J117" si="15">D67-I67</f>
         <v>-0.23902426331043003</v>
       </c>
       <c r="L67" s="5" t="str">
@@ -8670,11 +8670,11 @@
         <v/>
       </c>
       <c r="M67" s="5" t="str">
-        <f t="shared" ref="M67:M117" si="15">IF(D67&gt;=26,"Y","")</f>
+        <f t="shared" ref="M67:M117" si="16">IF(D67&gt;=26,"Y","")</f>
         <v/>
       </c>
       <c r="N67" s="5" t="str">
-        <f t="shared" ref="N67:N117" si="16">IF(L67&lt;&gt;M67,"Y","")</f>
+        <f t="shared" ref="N67:N117" si="17">IF(L67&lt;&gt;M67,"Y","")</f>
         <v/>
       </c>
     </row>
@@ -8692,23 +8692,23 @@
         <v>26.73</v>
       </c>
       <c r="E68" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.9299999999999997</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G68" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I68" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>26.683441986195962</v>
       </c>
       <c r="J68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.6558013804038012E-2</v>
       </c>
       <c r="L68" s="5" t="str">
@@ -8716,11 +8716,11 @@
         <v>Y</v>
       </c>
       <c r="M68" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Y</v>
       </c>
       <c r="N68" s="5" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
@@ -8738,23 +8738,23 @@
         <v>21.99</v>
       </c>
       <c r="E69" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G69" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I69" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>20.548068781554488</v>
       </c>
       <c r="J69" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.4419312184455109</v>
       </c>
       <c r="L69" s="5" t="str">
@@ -8762,11 +8762,11 @@
         <v/>
       </c>
       <c r="M69" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N69" s="5" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
@@ -8784,35 +8784,35 @@
         <v>30.81</v>
       </c>
       <c r="E70" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.41</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G70" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I70" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>31.797786066826632</v>
       </c>
       <c r="J70" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.98778606682663295</v>
       </c>
       <c r="L70" s="5" t="str">
-        <f t="shared" ref="L70:L117" si="17">IF(C70&gt;=28,"Y","")</f>
+        <f t="shared" ref="L70:L117" si="18">IF(C70&gt;=28,"Y","")</f>
         <v>Y</v>
       </c>
       <c r="M70" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Y</v>
       </c>
       <c r="N70" s="5" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
@@ -8830,35 +8830,35 @@
         <v>27.87</v>
       </c>
       <c r="E71" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.2099999999999973</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G71" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I71" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>27.98962338808365</v>
       </c>
       <c r="J71" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.11962338808364947</v>
       </c>
       <c r="L71" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M71" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N71" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M71" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N71" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -8876,35 +8876,35 @@
         <v>26.11</v>
       </c>
       <c r="E72" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.1400000000000006</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G72" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I72" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>27.226151160219722</v>
       </c>
       <c r="J72" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-1.1161511602197223</v>
       </c>
       <c r="L72" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M72" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N72" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M72" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N72" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -8922,35 +8922,35 @@
         <v>28.12</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.129999999999999</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G73" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I73" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28.145997217887107</v>
       </c>
       <c r="J73" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-2.5997217887105961E-2</v>
       </c>
       <c r="L73" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M73" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N73" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M73" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N73" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -8968,35 +8968,35 @@
         <v>24.05</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.5299999999999976</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G74" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.7296838714195886</v>
       </c>
       <c r="I74" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>23.85031612858041</v>
       </c>
       <c r="J74" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.19968387141959099</v>
       </c>
       <c r="L74" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M74" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N74" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M74" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N74" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9014,35 +9014,35 @@
         <v>28.83</v>
       </c>
       <c r="E75" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.5500000000000007</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G75" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I75" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28.265577205383867</v>
       </c>
       <c r="J75" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.56442279461613154</v>
       </c>
       <c r="L75" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M75" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N75" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M75" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N75" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9060,35 +9060,35 @@
         <v>24.17</v>
       </c>
       <c r="E76" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.1699999999999982</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G76" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I76" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24.549399132407626</v>
       </c>
       <c r="J76" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.3793991324076238</v>
       </c>
       <c r="L76" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M76" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N76" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M76" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N76" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9106,35 +9106,35 @@
         <v>13.06</v>
       </c>
       <c r="E77" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G77" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I77" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.333843486584724</v>
       </c>
       <c r="J77" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.72615651341527609</v>
       </c>
       <c r="L77" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M77" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N77" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M77" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N77" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9152,35 +9152,35 @@
         <v>22.28</v>
       </c>
       <c r="E78" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.3999999999999986</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G78" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I78" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>22.102608619012376</v>
       </c>
       <c r="J78" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.17739138098762552</v>
       </c>
       <c r="L78" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M78" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N78" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M78" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N78" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9198,35 +9198,35 @@
         <v>26.1</v>
       </c>
       <c r="E79" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.5199999999999996</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G79" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I79" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>26.646648143889266</v>
       </c>
       <c r="J79" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.5466481438892643</v>
       </c>
       <c r="L79" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M79" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N79" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M79" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N79" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9244,35 +9244,35 @@
         <v>17.579999999999998</v>
       </c>
       <c r="E80" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.0300000000000011</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G80" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I80" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18.358835164306107</v>
       </c>
       <c r="J80" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.77883516430610911</v>
       </c>
       <c r="L80" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M80" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N80" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M80" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N80" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9290,35 +9290,35 @@
         <v>29.98</v>
       </c>
       <c r="E81" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2199999999999989</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G81" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I81" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29.019850972671126</v>
       </c>
       <c r="J81" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.96014902732887464</v>
       </c>
       <c r="L81" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M81" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N81" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M81" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N81" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9336,35 +9336,35 @@
         <v>29</v>
       </c>
       <c r="E82" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.5199999999999996</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G82" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I82" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28.3943556534573</v>
       </c>
       <c r="J82" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.60564434654270016</v>
       </c>
       <c r="L82" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M82" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N82" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M82" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N82" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9382,35 +9382,35 @@
         <v>31.64</v>
       </c>
       <c r="E83" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.3500000000000014</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G83" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I83" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>31.586221473563135</v>
       </c>
       <c r="J83" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.3778526436865093E-2</v>
       </c>
       <c r="L83" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M83" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N83" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M83" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N83" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9428,35 +9428,35 @@
         <v>31.82</v>
       </c>
       <c r="E84" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.7299999999999969</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G84" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I84" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>31.181489208189483</v>
       </c>
       <c r="J84" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.63851079181051773</v>
       </c>
       <c r="L84" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M84" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N84" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M84" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N84" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9474,35 +9474,35 @@
         <v>30.18</v>
       </c>
       <c r="E85" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.0300000000000011</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G85" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I85" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29.948895490915188</v>
       </c>
       <c r="J85" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.23110450908481184</v>
       </c>
       <c r="L85" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M85" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N85" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M85" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N85" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9520,35 +9520,35 @@
         <v>29.46</v>
       </c>
       <c r="E86" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.9800000000000004</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G86" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I86" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29.240614026511299</v>
       </c>
       <c r="J86" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.21938597348870204</v>
       </c>
       <c r="L86" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M86" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N86" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M86" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N86" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9566,35 +9566,35 @@
         <v>29.25</v>
       </c>
       <c r="E87" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.6400000000000006</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G87" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I87" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28.734698694794236</v>
       </c>
       <c r="J87" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.51530130520576378</v>
       </c>
       <c r="L87" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M87" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N87" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M87" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N87" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9612,35 +9612,35 @@
         <v>31.74</v>
       </c>
       <c r="E88" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0199999999999996</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G88" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I88" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30.454810822632247</v>
       </c>
       <c r="J88" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.2851891773677515</v>
       </c>
       <c r="L88" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M88" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N88" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M88" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N88" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9658,35 +9658,35 @@
         <v>30.5</v>
       </c>
       <c r="E89" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.3200000000000003</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G89" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I89" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29.590155528424905</v>
       </c>
       <c r="J89" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.90984447157509507</v>
       </c>
       <c r="L89" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M89" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N89" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M89" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N89" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9704,35 +9704,35 @@
         <v>29.86</v>
       </c>
       <c r="E90" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.759999999999998</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G90" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I90" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30.326032374558814</v>
       </c>
       <c r="J90" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.46603237455881441</v>
       </c>
       <c r="L90" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M90" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N90" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M90" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N90" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9750,35 +9750,35 @@
         <v>33.46</v>
       </c>
       <c r="E91" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.9299999999999997</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G91" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I91" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33.793852011964866</v>
       </c>
       <c r="J91" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.33385201196486491</v>
       </c>
       <c r="L91" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M91" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N91" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M91" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N91" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9796,35 +9796,35 @@
         <v>32.950000000000003</v>
       </c>
       <c r="E92" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.519999999999996</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G92" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I92" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>32.947593638910867</v>
       </c>
       <c r="J92" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.4063610891360554E-3</v>
       </c>
       <c r="L92" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M92" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N92" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M92" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N92" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9842,35 +9842,35 @@
         <v>21.35</v>
       </c>
       <c r="E93" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.4599999999999973</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G93" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I93" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>22.222188606509135</v>
       </c>
       <c r="J93" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.87218860650913399</v>
       </c>
       <c r="L93" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M93" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N93" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M93" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N93" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9888,35 +9888,35 @@
         <v>20.170000000000002</v>
       </c>
       <c r="E94" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.7099999999999973</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G94" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I94" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>20.446885715211078</v>
       </c>
       <c r="J94" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.27688571521107619</v>
       </c>
       <c r="L94" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M94" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N94" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M94" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N94" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9934,35 +9934,35 @@
         <v>19.87</v>
       </c>
       <c r="E95" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.75</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G95" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I95" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>22.047417855552332</v>
       </c>
       <c r="J95" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-2.1774178555523314</v>
       </c>
       <c r="L95" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M95" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N95" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M95" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N95" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9980,35 +9980,35 @@
         <v>18.77</v>
       </c>
       <c r="E96" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G96" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I96" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19.425856591200279</v>
       </c>
       <c r="J96" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.65585659120027984</v>
       </c>
       <c r="L96" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M96" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N96" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M96" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N96" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10026,35 +10026,35 @@
         <v>18.25</v>
       </c>
       <c r="E97" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.57</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G97" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I97" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>21.311541009418423</v>
       </c>
       <c r="J97" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-3.0615410094184234</v>
       </c>
       <c r="L97" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M97" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N97" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M97" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N97" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10072,35 +10072,35 @@
         <v>26.94</v>
       </c>
       <c r="E98" s="1">
-        <f t="shared" ref="E98:E108" si="18">C98-D98</f>
+        <f t="shared" ref="E98:E108" si="19">C98-D98</f>
         <v>3.2799999999999976</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G98" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I98" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28.118401836157084</v>
       </c>
       <c r="J98" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-1.1784018361570823</v>
       </c>
       <c r="L98" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M98" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N98" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M98" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N98" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10118,35 +10118,35 @@
         <v>29.89</v>
       </c>
       <c r="E99" s="1">
+        <f t="shared" si="19"/>
+        <v>2.09</v>
+      </c>
+      <c r="F99" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G99" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="I99" s="1">
+        <f t="shared" si="14"/>
+        <v>29.737330897651688</v>
+      </c>
+      <c r="J99" s="1">
+        <f t="shared" si="15"/>
+        <v>0.15266910234831244</v>
+      </c>
+      <c r="L99" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>2.09</v>
-      </c>
-      <c r="F99" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G99" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I99" s="1">
-        <f t="shared" si="13"/>
-        <v>29.737330897651688</v>
-      </c>
-      <c r="J99" s="1">
-        <f t="shared" si="14"/>
-        <v>0.15266910234831244</v>
-      </c>
-      <c r="L99" s="5" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M99" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N99" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M99" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N99" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10164,35 +10164,35 @@
         <v>24.91</v>
       </c>
       <c r="E100" s="1">
+        <f t="shared" si="19"/>
+        <v>1.9299999999999997</v>
+      </c>
+      <c r="F100" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G100" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="I100" s="1">
+        <f t="shared" si="14"/>
+        <v>25.009322161241318</v>
+      </c>
+      <c r="J100" s="1">
+        <f t="shared" si="15"/>
+        <v>-9.9322161241317986E-2</v>
+      </c>
+      <c r="L100" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>1.9299999999999997</v>
-      </c>
-      <c r="F100" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G100" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I100" s="1">
-        <f t="shared" si="13"/>
-        <v>25.009322161241318</v>
-      </c>
-      <c r="J100" s="1">
-        <f t="shared" si="14"/>
-        <v>-9.9322161241317986E-2</v>
-      </c>
-      <c r="L100" s="5" t="str">
+        <v/>
+      </c>
+      <c r="M100" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N100" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M100" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N100" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10210,35 +10210,35 @@
         <v>24.63</v>
       </c>
       <c r="E101" s="1">
+        <f t="shared" si="19"/>
+        <v>1.1400000000000006</v>
+      </c>
+      <c r="F101" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G101" s="1">
+        <f t="shared" si="13"/>
+        <v>1.7449131204627868</v>
+      </c>
+      <c r="I101" s="1">
+        <f t="shared" si="14"/>
+        <v>24.025086879537213</v>
+      </c>
+      <c r="J101" s="1">
+        <f t="shared" si="15"/>
+        <v>0.60491312046278622</v>
+      </c>
+      <c r="L101" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>1.1400000000000006</v>
-      </c>
-      <c r="F101" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G101" s="1">
-        <f t="shared" si="12"/>
-        <v>1.7449131204627868</v>
-      </c>
-      <c r="I101" s="1">
-        <f t="shared" si="13"/>
-        <v>24.025086879537213</v>
-      </c>
-      <c r="J101" s="1">
-        <f t="shared" si="14"/>
-        <v>0.60491312046278622</v>
-      </c>
-      <c r="L101" s="5" t="str">
+        <v/>
+      </c>
+      <c r="M101" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N101" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M101" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N101" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10256,35 +10256,35 @@
         <v>22.76</v>
       </c>
       <c r="E102" s="1">
+        <f t="shared" si="19"/>
+        <v>0.41000000000000014</v>
+      </c>
+      <c r="F102" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G102" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="I102" s="1">
+        <f t="shared" si="14"/>
+        <v>21.63348712960201</v>
+      </c>
+      <c r="J102" s="1">
+        <f t="shared" si="15"/>
+        <v>1.1265128703979919</v>
+      </c>
+      <c r="L102" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>0.41000000000000014</v>
-      </c>
-      <c r="F102" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G102" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I102" s="1">
-        <f t="shared" si="13"/>
-        <v>21.63348712960201</v>
-      </c>
-      <c r="J102" s="1">
-        <f t="shared" si="14"/>
-        <v>1.1265128703979919</v>
-      </c>
-      <c r="L102" s="5" t="str">
+        <v/>
+      </c>
+      <c r="M102" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N102" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M102" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N102" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10302,35 +10302,35 @@
         <v>26.1</v>
       </c>
       <c r="E103" s="1">
+        <f t="shared" si="19"/>
+        <v>1.629999999999999</v>
+      </c>
+      <c r="F103" s="1">
+        <f t="shared" si="12"/>
+        <v>1.9020148474347067</v>
+      </c>
+      <c r="G103" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="I103" s="1">
+        <f t="shared" si="14"/>
+        <v>25.827985152565294</v>
+      </c>
+      <c r="J103" s="1">
+        <f t="shared" si="15"/>
+        <v>0.27201484743470772</v>
+      </c>
+      <c r="L103" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>1.629999999999999</v>
-      </c>
-      <c r="F103" s="1">
-        <f t="shared" si="11"/>
-        <v>1.9020148474347067</v>
-      </c>
-      <c r="G103" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I103" s="1">
-        <f t="shared" si="13"/>
-        <v>25.827985152565294</v>
-      </c>
-      <c r="J103" s="1">
-        <f t="shared" si="14"/>
-        <v>0.27201484743470772</v>
-      </c>
-      <c r="L103" s="5" t="str">
+        <v/>
+      </c>
+      <c r="M103" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N103" s="7" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M103" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N103" s="7" t="str">
-        <f t="shared" si="16"/>
         <v>Y</v>
       </c>
     </row>
@@ -10348,35 +10348,35 @@
         <v>24.05</v>
       </c>
       <c r="E104" s="1">
+        <f t="shared" si="19"/>
+        <v>6.5</v>
+      </c>
+      <c r="F104" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G104" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="I104" s="1">
+        <f t="shared" si="14"/>
+        <v>28.421951035187323</v>
+      </c>
+      <c r="J104" s="1">
+        <f t="shared" si="15"/>
+        <v>-4.3719510351873225</v>
+      </c>
+      <c r="L104" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>6.5</v>
-      </c>
-      <c r="F104" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G104" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I104" s="1">
-        <f t="shared" si="13"/>
-        <v>28.421951035187323</v>
-      </c>
-      <c r="J104" s="1">
-        <f t="shared" si="14"/>
-        <v>-4.3719510351873225</v>
-      </c>
-      <c r="L104" s="5" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M104" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N104" s="8" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M104" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N104" s="8" t="str">
-        <f t="shared" si="16"/>
         <v>Y</v>
       </c>
     </row>
@@ -10394,35 +10394,35 @@
         <v>26.64</v>
       </c>
       <c r="E105" s="1">
+        <f t="shared" si="19"/>
+        <v>3.2100000000000009</v>
+      </c>
+      <c r="F105" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G105" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="I105" s="1">
+        <f t="shared" si="14"/>
+        <v>27.778058794820154</v>
+      </c>
+      <c r="J105" s="1">
+        <f t="shared" si="15"/>
+        <v>-1.1380587948201537</v>
+      </c>
+      <c r="L105" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>3.2100000000000009</v>
-      </c>
-      <c r="F105" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G105" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I105" s="1">
-        <f t="shared" si="13"/>
-        <v>27.778058794820154</v>
-      </c>
-      <c r="J105" s="1">
-        <f t="shared" si="14"/>
-        <v>-1.1380587948201537</v>
-      </c>
-      <c r="L105" s="5" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M105" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N105" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M105" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N105" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10440,35 +10440,35 @@
         <v>27.46</v>
       </c>
       <c r="E106" s="1">
+        <f t="shared" si="19"/>
+        <v>3.7300000000000004</v>
+      </c>
+      <c r="F106" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G106" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="I106" s="1">
+        <f t="shared" si="14"/>
+        <v>29.010652512094453</v>
+      </c>
+      <c r="J106" s="1">
+        <f t="shared" si="15"/>
+        <v>-1.5506525120944517</v>
+      </c>
+      <c r="L106" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>3.7300000000000004</v>
-      </c>
-      <c r="F106" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G106" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I106" s="1">
-        <f t="shared" si="13"/>
-        <v>29.010652512094453</v>
-      </c>
-      <c r="J106" s="1">
-        <f t="shared" si="14"/>
-        <v>-1.5506525120944517</v>
-      </c>
-      <c r="L106" s="5" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M106" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N106" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M106" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N106" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10486,35 +10486,35 @@
         <v>28.89</v>
       </c>
       <c r="E107" s="1">
+        <f t="shared" si="19"/>
+        <v>3.009999999999998</v>
+      </c>
+      <c r="F107" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G107" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="I107" s="1">
+        <f t="shared" si="14"/>
+        <v>29.663743213038295</v>
+      </c>
+      <c r="J107" s="1">
+        <f t="shared" si="15"/>
+        <v>-0.77374321303829419</v>
+      </c>
+      <c r="L107" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>3.009999999999998</v>
-      </c>
-      <c r="F107" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G107" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I107" s="1">
-        <f t="shared" si="13"/>
-        <v>29.663743213038295</v>
-      </c>
-      <c r="J107" s="1">
-        <f t="shared" si="14"/>
-        <v>-0.77374321303829419</v>
-      </c>
-      <c r="L107" s="5" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M107" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N107" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M107" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N107" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10532,35 +10532,35 @@
         <v>21.88</v>
       </c>
       <c r="E108" s="1">
+        <f t="shared" si="19"/>
+        <v>0.92000000000000171</v>
+      </c>
+      <c r="F108" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G108" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="I108" s="1">
+        <f t="shared" si="14"/>
+        <v>21.293144088265073</v>
+      </c>
+      <c r="J108" s="1">
+        <f t="shared" si="15"/>
+        <v>0.58685591173492568</v>
+      </c>
+      <c r="L108" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>0.92000000000000171</v>
-      </c>
-      <c r="F108" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G108" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I108" s="1">
-        <f t="shared" si="13"/>
-        <v>21.293144088265073</v>
-      </c>
-      <c r="J108" s="1">
-        <f t="shared" si="14"/>
-        <v>0.58685591173492568</v>
-      </c>
-      <c r="L108" s="5" t="str">
+        <v/>
+      </c>
+      <c r="M108" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N108" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M108" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N108" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10578,35 +10578,35 @@
         <v>22.05</v>
       </c>
       <c r="E109" s="1">
-        <f t="shared" ref="E109:E117" si="19">C109-D109</f>
+        <f t="shared" ref="E109:E117" si="20">C109-D109</f>
         <v>1.1699999999999982</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G109" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I109" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>21.679479432485376</v>
       </c>
       <c r="J109" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.37052056751462459</v>
       </c>
       <c r="L109" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M109" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N109" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M109" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N109" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10624,35 +10624,35 @@
         <v>24.15</v>
       </c>
       <c r="E110" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.86000000000000298</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G110" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.683996124290001</v>
       </c>
       <c r="I110" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>23.326003875710001</v>
       </c>
       <c r="J110" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.82399612428999802</v>
       </c>
       <c r="L110" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M110" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N110" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M110" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N110" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10670,35 +10670,35 @@
         <v>22.61</v>
       </c>
       <c r="E111" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.2699999999999996</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G111" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I111" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>22.286577830545852</v>
       </c>
       <c r="J111" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.32342216945414748</v>
       </c>
       <c r="L111" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M111" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N111" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M111" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N111" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10716,35 +10716,35 @@
         <v>25.66</v>
       </c>
       <c r="E112" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.0599999999999987</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G112" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I112" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24.898940634321232</v>
       </c>
       <c r="J112" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.76105936567876853</v>
       </c>
       <c r="L112" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M112" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N112" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M112" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N112" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10762,35 +10762,35 @@
         <v>26.44</v>
       </c>
       <c r="E113" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.1600000000000001</v>
       </c>
       <c r="F113" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.8915948349314675</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I113" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>25.708405165068534</v>
       </c>
       <c r="J113" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.73159483493146737</v>
       </c>
       <c r="L113" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M113" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N113" s="7" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M113" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N113" s="7" t="str">
-        <f t="shared" si="16"/>
         <v>Y</v>
       </c>
     </row>
@@ -10808,35 +10808,35 @@
         <v>24.11</v>
       </c>
       <c r="E114" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.5800000000000018</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G114" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I114" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24.871345252591212</v>
       </c>
       <c r="J114" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.76134525259121233</v>
       </c>
       <c r="L114" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="M114" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N114" s="5" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="M114" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="N114" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10854,35 +10854,35 @@
         <v>27.13</v>
       </c>
       <c r="E115" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.9499999999999993</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G115" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I115" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>27.069777330416262</v>
       </c>
       <c r="J115" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6.0222669583737343E-2</v>
       </c>
       <c r="L115" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M115" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N115" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M115" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N115" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10900,35 +10900,35 @@
         <v>29.74</v>
       </c>
       <c r="E116" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.3399999999999999</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G116" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I116" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28.909469445751036</v>
       </c>
       <c r="J116" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.83053055424896272</v>
       </c>
       <c r="L116" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M116" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N116" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M116" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N116" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10946,35 +10946,35 @@
         <v>30.06</v>
       </c>
       <c r="E117" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.3300000000000018</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G117" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I117" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30.114467781295318</v>
       </c>
       <c r="J117" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-5.4467781295318929E-2</v>
       </c>
       <c r="L117" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>Y</v>
+      </c>
+      <c r="M117" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>Y</v>
+      </c>
+      <c r="N117" s="5" t="str">
         <f t="shared" si="17"/>
-        <v>Y</v>
-      </c>
-      <c r="M117" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>Y</v>
-      </c>
-      <c r="N117" s="5" t="str">
-        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -10998,16 +10998,16 @@
         <v>116</v>
       </c>
       <c r="F119" s="4">
-        <f t="shared" ref="F119:I119" si="20">COUNT(F$2:F$117)</f>
+        <f t="shared" ref="F119:I119" si="21">COUNT(F$2:F$117)</f>
         <v>10</v>
       </c>
       <c r="G119" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="H119" s="4"/>
       <c r="I119" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>116</v>
       </c>
       <c r="J119" s="4"/>

</xml_diff>

<commit_message>
Update UKWA percentile chart
</commit_message>
<xml_diff>
--- a/resources/ukwa/analysis/percentiles.xlsx
+++ b/resources/ukwa/analysis/percentiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wsw-results\resources\ukwa\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3AF855-EF60-4D54-955E-1CE60877740C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E297EC-12FA-4F30-9052-8137B0C04C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BC2B614C-97CE-4BFB-A796-CE0AF2755093}"/>
   </bookViews>
@@ -2185,8 +2185,8 @@
         <c:axId val="1231959152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="29"/>
-          <c:min val="27"/>
+          <c:max val="28"/>
+          <c:min val="26"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2305,8 +2305,8 @@
         <c:axId val="1230299248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="27"/>
-          <c:min val="25"/>
+          <c:max val="26"/>
+          <c:min val="24"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5528,8 +5528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF0D37A-FE3E-4993-BE94-996EF6CE4A41}">
   <dimension ref="A1:Y124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Further work on UKWA analysis - fix links to results.weymouthspeedweek.com
</commit_message>
<xml_diff>
--- a/resources/ukwa/analysis/percentiles.xlsx
+++ b/resources/ukwa/analysis/percentiles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wsw-results\resources\ukwa\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E297EC-12FA-4F30-9052-8137B0C04C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3504CC08-34C9-49E4-9C9E-84361A9724B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BC2B614C-97CE-4BFB-A796-CE0AF2755093}"/>
   </bookViews>
@@ -17,6 +17,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$117</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$2:$C$124</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$2:$D$124</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$2:$D$124</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$2:$D$124</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$D$2:$D$124</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3455,6 +3465,146 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Median Times for UKWA - 2010 to 2023</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Median Times for UKWA - 2010 to 2023</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{0C3C6711-4380-4A2A-9B4F-25CBC4A6D851}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:v>median</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binCount val="12"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+        <cx:numFmt formatCode="0.0" sourceLinked="0"/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>25th Percentile for UKWA - 2010 to 2023</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>25th Percentile for UKWA - 2010 to 2023</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{0C3C6711-4380-4A2A-9B4F-25CBC4A6D851}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:v>25th percentile</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binCount val="12"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+        <cx:numFmt formatCode="0.0" sourceLinked="0"/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3575,6 +3725,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5106,6 +5336,1022 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -5226,13 +6472,169 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B1D035B-81A2-4CA4-9AFF-FD1488D4A96B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10801349" y="13525500"/>
+              <a:ext cx="6696075" cy="3695700"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Chart 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BCEF1ED-E10B-471F-A37F-792DD58CD3C5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10801350" y="17526000"/>
+              <a:ext cx="6696075" cy="3695700"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5270,7 +6672,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5376,7 +6778,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5518,7 +6920,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5528,8 +6930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF0D37A-FE3E-4993-BE94-996EF6CE4A41}">
   <dimension ref="A1:Y124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="N92" sqref="N92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add r-squared to analysis
</commit_message>
<xml_diff>
--- a/resources/ukwa/analysis/percentiles.xlsx
+++ b/resources/ukwa/analysis/percentiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wsw-results\resources\ukwa\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3504CC08-34C9-49E4-9C9E-84361A9724B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52451064-4A49-46B2-86B9-1A2EEFA310EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BC2B614C-97CE-4BFB-A796-CE0AF2755093}"/>
   </bookViews>
@@ -21,12 +21,6 @@
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$2:$C$124</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$D$1</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$2:$D$124</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$2:$D$124</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$2:$D$124</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$D$2:$D$124</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -326,8 +320,44 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.4241989478718323E-2"/>
+                  <c:y val="8.4399541121386971E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1462,8 +1492,44 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.18406504065040649"/>
+                  <c:y val="2.0411520228647485E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -3470,7 +3536,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3508,7 +3574,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{0C3C6711-4380-4A2A-9B4F-25CBC4A6D851}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>median</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6930,8 +6996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF0D37A-FE3E-4993-BE94-996EF6CE4A41}">
   <dimension ref="A1:Y124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="N92" sqref="N92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>